<commit_message>
Alterações de validação no DashBoard
</commit_message>
<xml_diff>
--- a/Site Estático/Dashboard/Métricas.xlsx
+++ b/Site Estático/Dashboard/Métricas.xlsx
@@ -5,23 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gibie\OneDrive\Área de Trabalho\SPTECH\Primeiro Semestre\Pesquisa e Inovação\SPRINT 2\BrightSight\Bright Sight (GIT-HUB)\BrightSight\Site Estático\Dashboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gibie\OneDrive\Área de Trabalho\SPTECH\Primeiro Semestre\Pesquisa e Inovação\SPRINT 2\BrightSight\Site Estático (pessoal)\Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3966C0EA-9650-419C-86F8-EF1420B9AED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6F3135-72B3-4560-9515-6D5506866D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{13C4CB50-7179-4ACF-9002-4FBE8A0C6770}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{13C4CB50-7179-4ACF-9002-4FBE8A0C6770}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v5.0" hidden="1">Planilha2!$C$1</definedName>
-    <definedName name="_xlchart.v5.1" hidden="1">Planilha2!$C$17</definedName>
-    <definedName name="_xlchart.v5.2" hidden="1">Planilha2!$D$17:$E$17</definedName>
-    <definedName name="_xlchart.v5.3" hidden="1">Planilha2!$D$1:$E$1</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="12">
   <si>
     <t>Data</t>
   </si>
@@ -160,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -188,6 +182,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -289,7 +284,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>IDEAL</c:v>
+                  <c:v>REAL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -424,7 +419,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>REAL</c:v>
+                  <c:v>IDEAL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -987,6 +982,777 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Evolução da Incidência Solar por Sensor</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>REAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Planilha2!$C$30:$C$43</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29166666666666702</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33333333333333398</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.41666666666666702</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45833333333333398</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.54166666666666663</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.58333333333333603</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.625000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.66666666666666996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.70833333333333703</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.750000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.79166666666667096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$D$30:$D$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2221-4525-A938-153D942E16B1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Planilha2!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IDEAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Planilha2!$C$30:$C$43</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29166666666666702</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33333333333333398</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.41666666666666702</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45833333333333398</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.54166666666666663</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.58333333333333603</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.625000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.66666666666666996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.70833333333333703</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.750000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.79166666666667096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Planilha2!$E$30:$E$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2221-4525-A938-153D942E16B1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:dropLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                  <a:alpha val="33000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:dropLines>
+        <c:smooth val="0"/>
+        <c:axId val="2062645759"/>
+        <c:axId val="2062626559"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2062645759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2062626559"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2062626559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2062645759"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>(Planilha2!$D$29,Planilha2!$E$29)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>IDEAL</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>REAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Planilha2!$D$44,Planilha2!$E$44)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6070</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6785</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D203-4034-8F79-A37C3D5A2617}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1067,6 +1833,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
   <cs:axisTitle>
@@ -1606,6 +2452,1063 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="20" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+            <a:alpha val="33000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2193,6 +4096,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>13223</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8B4296E-F1D2-45A6-9CA6-8A316AAF16BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>602673</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>69274</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Gráfico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D163415-6900-7921-FF5E-F393C2FA7FB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2693,10 +4670,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3031C96B-8DEF-4149-B011-FBCF3BA6A9EF}">
-  <dimension ref="C1:U50"/>
+  <dimension ref="C1:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E44" activeCellId="1" sqref="D44 E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2726,10 +4703,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -3003,102 +4980,294 @@
       <c r="P27" s="8"/>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="I28" s="4"/>
-      <c r="J28" s="3"/>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="I29" s="4"/>
-      <c r="J29" s="3"/>
+      <c r="C29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="I30" s="4"/>
-      <c r="J30" s="3"/>
+      <c r="C30" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="D30" s="3">
+        <v>150</v>
+      </c>
+      <c r="E30">
+        <v>185</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J30" s="12"/>
+      <c r="L30" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="M30" s="12"/>
+      <c r="O30" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="P30" s="12"/>
     </row>
     <row r="31" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="I31" s="4"/>
-      <c r="J31" s="3"/>
+      <c r="C31" s="4">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="D31" s="3">
+        <v>180</v>
+      </c>
+      <c r="E31">
+        <v>200</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" s="10">
+        <f>D44/14</f>
+        <v>433.57142857142856</v>
+      </c>
+      <c r="K31" s="13">
+        <f>J32-J31</f>
+        <v>51.071428571428612</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M31" s="5">
+        <f>MAX(D30:D43)</f>
+        <v>650</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P31" s="5">
+        <f>MAX(D30:D43) - MIN(D30:D43)</f>
+        <v>550</v>
+      </c>
     </row>
     <row r="32" spans="3:16" x14ac:dyDescent="0.3">
-      <c r="I32" s="4"/>
-      <c r="J32" s="3"/>
+      <c r="C32" s="4">
+        <v>0.33333333333333398</v>
+      </c>
+      <c r="D32" s="3">
+        <v>300</v>
+      </c>
+      <c r="E32">
+        <v>340</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J32" s="11">
+        <f>E44/14</f>
+        <v>484.64285714285717</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M32" s="7">
+        <f>MAX(E30:E43)</f>
+        <v>750</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P32" s="6">
+        <f>MAX(E30:E43) - MIN(E30:E43)</f>
+        <v>600</v>
+      </c>
     </row>
-    <row r="33" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I33" s="4"/>
-      <c r="J33" s="3"/>
+    <row r="33" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C33" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D33" s="3">
+        <v>450</v>
+      </c>
+      <c r="E33">
+        <v>520</v>
+      </c>
+      <c r="T33" s="8"/>
     </row>
-    <row r="34" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I34" s="4"/>
-      <c r="J34" s="3"/>
+    <row r="34" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C34" s="4">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="D34" s="3">
+        <v>460</v>
+      </c>
+      <c r="E34">
+        <v>480</v>
+      </c>
+      <c r="K34" s="8"/>
+      <c r="N34" s="8"/>
     </row>
-    <row r="35" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I35" s="4"/>
-      <c r="J35" s="3"/>
+    <row r="35" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C35" s="4">
+        <v>0.45833333333333398</v>
+      </c>
+      <c r="D35" s="3">
+        <v>510</v>
+      </c>
+      <c r="E35">
+        <v>550</v>
+      </c>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I36" s="4"/>
-      <c r="J36" s="3"/>
+    <row r="36" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C36" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="3">
+        <v>580</v>
+      </c>
+      <c r="E36">
+        <v>710</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I37" s="4"/>
-      <c r="J37" s="3"/>
+    <row r="37" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C37" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D37" s="3">
+        <v>630</v>
+      </c>
+      <c r="E37">
+        <v>750</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I38" s="4"/>
-      <c r="J38" s="3"/>
+    <row r="38" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C38" s="4">
+        <v>0.58333333333333603</v>
+      </c>
+      <c r="D38" s="3">
+        <v>650</v>
+      </c>
+      <c r="E38">
+        <v>700</v>
+      </c>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I39" s="4"/>
-      <c r="J39" s="3"/>
+    <row r="39" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C39" s="4">
+        <v>0.625000000000003</v>
+      </c>
+      <c r="D39" s="3">
+        <v>610</v>
+      </c>
+      <c r="E39">
+        <v>640</v>
+      </c>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I40" s="4"/>
-      <c r="J40" s="3"/>
+    <row r="40" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C40" s="4">
+        <v>0.66666666666666996</v>
+      </c>
+      <c r="D40" s="3">
+        <v>570</v>
+      </c>
+      <c r="E40">
+        <v>610</v>
+      </c>
+      <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I41" s="4"/>
-      <c r="J41" s="3"/>
+    <row r="41" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C41" s="4">
+        <v>0.70833333333333703</v>
+      </c>
+      <c r="D41" s="3">
+        <v>530</v>
+      </c>
+      <c r="E41">
+        <v>550</v>
+      </c>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I42" s="4"/>
-      <c r="J42" s="3"/>
+    <row r="42" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C42" s="4">
+        <v>0.750000000000004</v>
+      </c>
+      <c r="D42" s="3">
+        <v>350</v>
+      </c>
+      <c r="E42">
+        <v>400</v>
+      </c>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I43" s="4"/>
-      <c r="J43" s="3"/>
+    <row r="43" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C43" s="4">
+        <v>0.79166666666667096</v>
+      </c>
+      <c r="D43" s="3">
+        <v>100</v>
+      </c>
+      <c r="E43">
+        <v>150</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I44" s="4"/>
-      <c r="J44" s="3"/>
+    <row r="44" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C44" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="3">
+        <f>SUM(D30:D43)</f>
+        <v>6070</v>
+      </c>
+      <c r="E44">
+        <f>SUM(E30:E43)</f>
+        <v>6785</v>
+      </c>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I45" s="4"/>
-      <c r="J45" s="3"/>
+    <row r="45" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C45" s="4"/>
+      <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I46" s="4"/>
-      <c r="J46" s="3"/>
+    <row r="46" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C46" s="4"/>
+      <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I47" s="4"/>
-      <c r="J47" s="3"/>
-    </row>
-    <row r="48" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I48" s="4"/>
-      <c r="J48" s="3"/>
-    </row>
-    <row r="49" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I49" s="4"/>
-      <c r="J49" s="3"/>
-    </row>
-    <row r="50" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I50" s="4"/>
-      <c r="J50" s="3"/>
+    <row r="47" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C47" s="4"/>
+      <c r="D47" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="O3:P3"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="O30:P30"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>